<commit_message>
Improve Employee Roster quick edit UX
1. Add specific success alerts showing what was saved:
   - 'Added: John Smith'
   - 'Terminated: Jane Doe (2024-11-30)'
   - 'Transferred: Bob → Sales & Marketing'

2. Department field is now a dropdown with options:
   - COGS Support
   - COGS Onboarding
   - COGS Prof. Services
   - Sales & Marketing
   - Marketing
   - Client Success
   - Research & Development
   - General & Administrative

3. Fixed event listeners for select elements (change vs input)
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C84C52-DAAC-5042-B5B5-3E7E0CCF46BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21418663-1392-0B40-BC33-5508C2DC45AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="11" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="11" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_Homepage" sheetId="2" state="hidden" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="PR_JE_Draft" sheetId="14" r:id="rId13"/>
     <sheet name="PR_Archive_Summary" sheetId="15" r:id="rId14"/>
     <sheet name="PR_Expense_Mapping" sheetId="16" r:id="rId15"/>
-    <sheet name="SS_Employee_Roster" sheetId="17" state="hidden" r:id="rId16"/>
+    <sheet name="SS_Employee_Roster" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="743">
   <si>
     <t>ForgeSuite</t>
   </si>
@@ -2290,7 +2290,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2536,10 +2536,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2553,19 +2553,19 @@
     <xf numFmtId="15" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2594,30 +2594,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2719,6 +2695,126 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
@@ -2738,9 +2834,6 @@
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2836,100 +2929,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2974,7 +2974,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D1A9EEA6-D00F-584C-9188-148053B4AAE3}" name="Category"/>
     <tableColumn id="2" xr3:uid="{451E6C72-2FF9-794A-AEBF-C614403C97CC}" name="Field"/>
-    <tableColumn id="3" xr3:uid="{B58603AA-D6E7-E64C-8984-DB17B7DD5145}" name="Value" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B58603AA-D6E7-E64C-8984-DB17B7DD5145}" name="Value" dataDxfId="35"/>
     <tableColumn id="4" xr3:uid="{5E937999-FA47-5043-99D8-6164C7566D76}" name="Permanent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2982,21 +2982,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{E1AC754E-D7B1-7547-B155-E319972EBD10}" name="PR_Expense_Mapping" displayName="PR_Expense_Mapping" ref="A1:E97" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{E1AC754E-D7B1-7547-B155-E319972EBD10}" name="PR_Expense_Mapping" displayName="PR_Expense_Mapping" ref="A1:E97" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:E97" xr:uid="{E1AC754E-D7B1-7547-B155-E319972EBD10}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9A0961C9-FB60-CF4C-98CD-3400453E97BD}" name="Department Name"/>
-    <tableColumn id="2" xr3:uid="{CC9424B7-8BBB-DA45-A580-7106F5E3DBD0}" name="Account Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{682A51A4-7D5D-924A-A888-71E55BD9FFB7}" name="Payroll Category" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{61CE82C1-A317-FA4C-B8F7-8687CAD362A5}" name="Account Number" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{A678014E-AD9A-D448-9C24-033C2399D068}" name="Expense Review" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{CC9424B7-8BBB-DA45-A580-7106F5E3DBD0}" name="Account Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{682A51A4-7D5D-924A-A888-71E55BD9FFB7}" name="Payroll Category" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{61CE82C1-A317-FA4C-B8F7-8687CAD362A5}" name="Account Number" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A678014E-AD9A-D448-9C24-033C2399D068}" name="Expense Review" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3514F8D-9142-E34B-B630-045E1122CAEC}" name="SS_Chart_of_Accounts" displayName="SS_Chart_of_Accounts" ref="A1:D327" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3514F8D-9142-E34B-B630-045E1122CAEC}" name="SS_Chart_of_Accounts" displayName="SS_Chart_of_Accounts" ref="A1:D327" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:D327" xr:uid="{C3514F8D-9142-E34B-B630-045E1122CAEC}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{149761D8-036D-A14B-BB8A-345889815318}" name="Account_Number"/>
@@ -3009,39 +3009,39 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9AF2CAC0-544E-5E45-8D2B-A31076DEB4A1}" name="PTO_Data" displayName="PTO_Data" ref="A1:N38" totalsRowShown="0" headerRowDxfId="34" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9AF2CAC0-544E-5E45-8D2B-A31076DEB4A1}" name="PTO_Data" displayName="PTO_Data" ref="A1:N38" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:N38" xr:uid="{9AF2CAC0-544E-5E45-8D2B-A31076DEB4A1}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{3C09C68D-80EF-0847-90CB-A3926352912F}" name="Company Name" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{F7F9927B-CA5A-C340-A006-BE67CDBBD2CF}" name="Form Name" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{FD8C98C4-CFF8-2348-9AC1-E559B81091A6}" name="Selection Criteria" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F64C3A48-E5CF-6A48-A55F-4A0B03105F86}" name="Employee Name" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{9E27D7B3-5737-3942-ADB1-FB8E8EE703DA}" name="Accrue Thru Date" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{C13E65F1-CDFC-3F4A-A0C9-102E660E266F}" name="Year Ending" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{4F9FD05C-304F-B747-BBE3-2F38CF72E3B3}" name="Plan Description" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{A42CDA81-B29F-BB43-B120-7221654145BD}" name="Accrual Rate" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{DC905EF4-C214-AE45-8C38-11395EB567EC}" name="Carry Over" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{C309AAA0-4BC1-CB47-90F0-681120BE6534}" name="Pay Period Accrued" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{5BF1C369-E8E5-F645-B17F-B43B03A983D9}" name="Pay Period Used" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C13D5914-8F00-8749-9231-4B0FC1DF80D4}" name="YTD Accrued" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{0AE9DA03-5102-B24A-8060-FFE7E1C7C1B0}" name="YTD Used" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{B408FCEA-58F8-AB42-B31E-1B26BD4ACFBB}" name="Balance" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3C09C68D-80EF-0847-90CB-A3926352912F}" name="Company Name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{F7F9927B-CA5A-C340-A006-BE67CDBBD2CF}" name="Form Name" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{FD8C98C4-CFF8-2348-9AC1-E559B81091A6}" name="Selection Criteria" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{F64C3A48-E5CF-6A48-A55F-4A0B03105F86}" name="Employee Name" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{9E27D7B3-5737-3942-ADB1-FB8E8EE703DA}" name="Accrue Thru Date" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{C13E65F1-CDFC-3F4A-A0C9-102E660E266F}" name="Year Ending" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{4F9FD05C-304F-B747-BBE3-2F38CF72E3B3}" name="Plan Description" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{A42CDA81-B29F-BB43-B120-7221654145BD}" name="Accrual Rate" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{DC905EF4-C214-AE45-8C38-11395EB567EC}" name="Carry Over" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{C309AAA0-4BC1-CB47-90F0-681120BE6534}" name="Pay Period Accrued" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{5BF1C369-E8E5-F645-B17F-B43B03A983D9}" name="Pay Period Used" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C13D5914-8F00-8749-9231-4B0FC1DF80D4}" name="YTD Accrued" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{0AE9DA03-5102-B24A-8060-FFE7E1C7C1B0}" name="YTD Used" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{B408FCEA-58F8-AB42-B31E-1B26BD4ACFBB}" name="Balance" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F37D8B6-238C-3A40-8D44-06B270BD489B}" name="PTO_JE_Draft" displayName="PTO_JE_Draft" ref="A1:I3" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F37D8B6-238C-3A40-8D44-06B270BD489B}" name="PTO_JE_Draft" displayName="PTO_JE_Draft" ref="A1:I3" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:I3" xr:uid="{6F37D8B6-238C-3A40-8D44-06B270BD489B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DCC0AE7D-B5DB-644B-A2BC-A861DC4C3816}" name="RefNumber"/>
     <tableColumn id="2" xr3:uid="{9EC82BE6-A81E-9142-B356-BE23E3AE7533}" name="TxnDate"/>
     <tableColumn id="3" xr3:uid="{49C016C3-B3E6-C74F-A4F9-C62031B96D10}" name="Account Number"/>
     <tableColumn id="4" xr3:uid="{B74E3BE6-CA2E-0D44-A061-632A9F864ABC}" name="Account Name"/>
-    <tableColumn id="5" xr3:uid="{2B3FB472-AEF1-A14F-A762-FD305B4DF368}" name="LineAmount" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{78722B56-5DBC-7E41-938C-087DADE7D092}" name="Debit" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{E44A96F3-B513-0447-A703-BF0C91CA18A8}" name="Credit" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2B3FB472-AEF1-A14F-A762-FD305B4DF368}" name="LineAmount" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{78722B56-5DBC-7E41-938C-087DADE7D092}" name="Debit" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{E44A96F3-B513-0447-A703-BF0C91CA18A8}" name="Credit" dataDxfId="14"/>
     <tableColumn id="8" xr3:uid="{E727F5EE-3438-8B43-8417-5AF26FC11C54}" name="LineDesc"/>
     <tableColumn id="9" xr3:uid="{FBCCC04B-7144-7E40-8C4B-D70E0956EA4D}" name="Department"/>
   </tableColumns>
@@ -3050,7 +3050,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{487BD7F1-01B6-944A-94C3-24ECB83D6B56}" name="PTO_Archive_Summary" displayName="PTO_Archive_Summary" ref="A1:G2" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{487BD7F1-01B6-944A-94C3-24ECB83D6B56}" name="PTO_Archive_Summary" displayName="PTO_Archive_Summary" ref="A1:G2" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:G2" xr:uid="{487BD7F1-01B6-944A-94C3-24ECB83D6B56}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C0474DB5-8606-A647-8E54-EDD8C126FB55}" name="Analysis Date"/>
@@ -3066,7 +3066,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5206E609-460B-8449-AFB6-2193E6C3C990}" name="PR_Data" displayName="PR_Data" ref="A1:T54" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5206E609-460B-8449-AFB6-2193E6C3C990}" name="PR_Data" displayName="PR_Data" ref="A1:T54" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:T54" xr:uid="{5206E609-460B-8449-AFB6-2193E6C3C990}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{C8472340-B63B-4F4D-92E0-37936BA35D1B}" name="Company Name"/>
@@ -3095,7 +3095,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D9C94DF4-0D0D-384B-BF54-026F663A5597}" name="PR_Data_Clean" displayName="PR_Data_Clean" ref="A1:H211" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D9C94DF4-0D0D-384B-BF54-026F663A5597}" name="PR_Data_Clean" displayName="PR_Data_Clean" ref="A1:H211" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:H211" xr:uid="{D9C94DF4-0D0D-384B-BF54-026F663A5597}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0E30CFDA-EFA0-394D-B9CE-C3BF448A9A2F}" name="Payroll Date"/>
@@ -3112,16 +3112,16 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{94555BAA-07E3-964C-A848-BCA9059C0900}" name="PR_JE_Draft" displayName="PR_JE_Draft" ref="A1:I46" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{94555BAA-07E3-964C-A848-BCA9059C0900}" name="PR_JE_Draft" displayName="PR_JE_Draft" ref="A1:I46" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:I46" xr:uid="{94555BAA-07E3-964C-A848-BCA9059C0900}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{56E976ED-E26A-274C-AABF-0EFE9B9B0E75}" name="RefNumber"/>
-    <tableColumn id="2" xr3:uid="{354D36E0-A329-8E4C-A37E-B4877DDF49EB}" name="TxnDate" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{354D36E0-A329-8E4C-A37E-B4877DDF49EB}" name="TxnDate" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{044E1D5A-8569-FB4F-A904-1BE2CA69BA82}" name="Account Number"/>
     <tableColumn id="4" xr3:uid="{199408DD-165A-CC49-91AD-DBCD5617B6DF}" name="Account Name"/>
-    <tableColumn id="5" xr3:uid="{4DF32A67-FB0B-2A47-A746-9CBE69D1DB63}" name="LineAmount" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4766A28F-3CBE-9C40-B576-3B44B8036F7B}" name="Debit" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{0CF4FF6C-212A-FF4B-9004-5D02275CB4B6}" name="Credit" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{4DF32A67-FB0B-2A47-A746-9CBE69D1DB63}" name="LineAmount" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{4766A28F-3CBE-9C40-B576-3B44B8036F7B}" name="Debit" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{0CF4FF6C-212A-FF4B-9004-5D02275CB4B6}" name="Credit" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{DAA3DA61-1DB2-154D-BA4A-8F1FA4104B84}" name="LineDesc"/>
     <tableColumn id="9" xr3:uid="{B68DF95B-18F7-A747-ACA3-829FC52A9E4B}" name="Department"/>
   </tableColumns>
@@ -3130,7 +3130,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{BA990B64-D6F5-724F-B330-8F617FB33C11}" name="PR_Archive_Summary" displayName="PR_Archive_Summary" ref="A1:H2" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{BA990B64-D6F5-724F-B330-8F617FB33C11}" name="PR_Archive_Summary" displayName="PR_Archive_Summary" ref="A1:H2" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:H2" xr:uid="{BA990B64-D6F5-724F-B330-8F617FB33C11}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4AD44A89-4D16-4647-AE61-DEE774C748EE}" name="Payroll Date"/>
@@ -17720,13 +17720,19 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C005F75D-EC6D-BC43-BB10-984F5A7D9616}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>41</v>
       </c>
@@ -17746,7 +17752,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>440</v>
       </c>
@@ -17754,7 +17760,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>442</v>
       </c>
@@ -17762,7 +17768,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>444</v>
       </c>
@@ -17770,7 +17776,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>445</v>
       </c>
@@ -17778,7 +17784,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>447</v>
       </c>
@@ -17786,7 +17792,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>448</v>
       </c>
@@ -17794,7 +17800,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>449</v>
       </c>
@@ -17802,7 +17808,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>451</v>
       </c>
@@ -17810,7 +17816,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>452</v>
       </c>
@@ -17818,7 +17824,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>453</v>
       </c>
@@ -17826,7 +17832,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>454</v>
       </c>
@@ -17834,71 +17840,95 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>455</v>
       </c>
       <c r="B13" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>456</v>
       </c>
       <c r="B14" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>457</v>
       </c>
       <c r="B15" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>458</v>
       </c>
       <c r="B16" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>459</v>
       </c>
       <c r="B17" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>460</v>
       </c>
       <c r="B18" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>461</v>
       </c>
       <c r="B19" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>463</v>
       </c>
       <c r="B20" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>464</v>
       </c>
@@ -17906,7 +17936,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>465</v>
       </c>
@@ -17914,7 +17944,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>466</v>
       </c>
@@ -17922,7 +17952,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>467</v>
       </c>
@@ -17930,7 +17960,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>468</v>
       </c>
@@ -17938,7 +17968,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>469</v>
       </c>
@@ -17946,7 +17976,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>470</v>
       </c>
@@ -17954,7 +17984,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>471</v>
       </c>
@@ -17962,7 +17992,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>472</v>
       </c>
@@ -17970,7 +18000,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>473</v>
       </c>
@@ -17978,7 +18008,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>474</v>
       </c>
@@ -17986,7 +18016,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>475</v>
       </c>
@@ -17994,7 +18024,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>476</v>
       </c>
@@ -18002,7 +18032,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>477</v>
       </c>
@@ -18010,7 +18040,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>478</v>
       </c>
@@ -18018,7 +18048,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>479</v>
       </c>
@@ -18026,13 +18056,16 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>480</v>
       </c>
       <c r="B37" t="s">
         <v>166</v>
       </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve archive UX for Excel Desktop
- Show warning message when steps are incomplete
- Add try/catch with visible error alerts
- Remove console.log (not visible in desktop)
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21418663-1392-0B40-BC33-5508C2DC45AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109B64D-B400-8C4F-8565-8FE802BBD2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="11" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="743">
   <si>
     <t>ForgeSuite</t>
   </si>
@@ -14113,7 +14113,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14525,7 +14525,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="52" t="s">
         <v>656</v>
       </c>
@@ -15996,7 +15996,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16051,14 +16051,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21" style="19" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -17720,10 +17720,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C005F75D-EC6D-BC43-BB10-984F5A7D9616}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H20"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17732,7 +17732,7 @@
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>41</v>
       </c>
@@ -17752,7 +17752,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>440</v>
       </c>
@@ -17760,7 +17760,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>442</v>
       </c>
@@ -17768,7 +17768,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>444</v>
       </c>
@@ -17776,7 +17776,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>445</v>
       </c>
@@ -17784,7 +17784,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>447</v>
       </c>
@@ -17792,7 +17792,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>448</v>
       </c>
@@ -17800,7 +17800,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>449</v>
       </c>
@@ -17808,7 +17808,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>451</v>
       </c>
@@ -17816,7 +17816,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>452</v>
       </c>
@@ -17824,7 +17824,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>453</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>454</v>
       </c>
@@ -17840,95 +17840,71 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>455</v>
       </c>
       <c r="B13" t="s">
         <v>450</v>
       </c>
-      <c r="H13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>456</v>
       </c>
       <c r="B14" t="s">
         <v>450</v>
       </c>
-      <c r="H14" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>457</v>
       </c>
       <c r="B15" t="s">
         <v>450</v>
       </c>
-      <c r="H15" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>458</v>
       </c>
       <c r="B16" t="s">
         <v>450</v>
       </c>
-      <c r="H16" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>459</v>
       </c>
       <c r="B17" t="s">
         <v>450</v>
       </c>
-      <c r="H17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>460</v>
       </c>
       <c r="B18" t="s">
         <v>238</v>
       </c>
-      <c r="H18" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>461</v>
       </c>
       <c r="B19" t="s">
         <v>462</v>
       </c>
-      <c r="H19" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>463</v>
       </c>
       <c r="B20" t="s">
         <v>462</v>
       </c>
-      <c r="H20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>464</v>
       </c>
@@ -17936,7 +17912,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>465</v>
       </c>
@@ -17944,7 +17920,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>466</v>
       </c>
@@ -17952,7 +17928,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>467</v>
       </c>
@@ -17960,7 +17936,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>468</v>
       </c>
@@ -17968,7 +17944,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>469</v>
       </c>
@@ -17976,7 +17952,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>470</v>
       </c>
@@ -17984,7 +17960,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>471</v>
       </c>
@@ -17992,7 +17968,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>472</v>
       </c>
@@ -18000,7 +17976,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>473</v>
       </c>
@@ -18008,7 +17984,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>474</v>
       </c>
@@ -18016,7 +17992,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>475</v>
       </c>
@@ -18077,7 +18053,7 @@
   <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix archive button click - use onclick and clone to ensure handler fires
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109B64D-B400-8C4F-8565-8FE802BBD2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078C55C5-AEAD-AB4D-9C16-A729A5277FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="11" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_Homepage" sheetId="2" state="hidden" r:id="rId1"/>
@@ -14111,7 +14111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC6B1F-6222-ED4D-B97D-0285FC663B78}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
@@ -18052,9 +18052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF3CE7-E34E-044F-A5DE-BB3AC931C52F}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fix archive button - use inline onclick with global handler
Event listeners weren't binding properly, so switched to inline onclick
with a global window.handleArchiveClick function that shows immediate
feedback and calls handleArchiveRun
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078C55C5-AEAD-AB4D-9C16-A729A5277FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7ED7E-A0CE-E745-81B7-0803F6C5FB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
@@ -14113,7 +14113,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14722,7 +14722,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18052,7 +18052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF3CE7-E34E-044F-A5DE-BB3AC931C52F}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Replace window.alert/confirm with Office-safe toast notifications
window.alert and window.confirm are not supported in Office Add-ins on
Excel Desktop. Created showToast() and showConfirm() helper functions that
display styled in-panel notifications and confirmation dialogs instead.
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7ED7E-A0CE-E745-81B7-0803F6C5FB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233DBB70-B111-2A42-A8F0-6553CE9A3DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
@@ -18052,9 +18052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF3CE7-E34E-044F-A5DE-BB3AC931C52F}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Bi-directional sync between Excel tabs and side panel
- Added SHEET_TO_STEP_MAP reverse lookup
- Registered worksheet onActivated event listener
- When user manually switches Excel tabs, side panel updates to match:
  • PR_Homepage → Home view
  • PR_Data → Step 1 (Import)
  • PR_Data_Clean → Step 3 (Validate)
  • PR_Expense_Review → Step 4 (Expense Review)
  • PR_JE_Draft → Step 5 (Journal Entry)
  • PR_Archive_Summary → Step 6 (Archive)
  • SS_PF_Config → Step 0 (Configuration)
  • SS_Employee_Roster → Step 2 (Headcount)
- Prevents activation loop by checking if step changed
- Triggers step initialization when needed (e.g., headcount analysis)
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E18B93-D348-FB4F-9B76-9537866461A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B755F7-5F1F-8F46-8CB8-FE465B6AC86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="14" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_Homepage" sheetId="2" state="hidden" r:id="rId1"/>
@@ -6015,7 +6015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:S52"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25109,8 +25109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED097E2E-4604-594C-9471-1C4F0F3FB56C}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -27112,9 +27112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF3CE7-E34E-044F-A5DE-BB3AC931C52F}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Add bi-directional tab sync to PTO module
- Added STEP_SHEET_MAP for step → sheet mapping
- Added SHEET_TO_STEP_MAP for sheet → step mapping (reverse lookup)
- Registered worksheet onActivated event listener
- When user manually switches Excel tabs, side panel updates to match:
  • PTO_Homepage → Step 0 (Configuration)
  • PTO_Data → Step 1 (Import)
  • PTO_Analysis → Step 4 (Accrual Review)
  • PTO_JE_Draft → Step 5 (Journal Entry)
  • SS_Employee_Roster → Step 2 (Headcount)
- Refactored focusStep() to use STEP_SHEET_MAP consistently
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B755F7-5F1F-8F46-8CB8-FE465B6AC86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343E273B-6D49-684F-A519-5FF0503552AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
@@ -3172,7 +3172,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="1" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -6015,7 +6015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:C25"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="A15:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7018,20 +7018,13 @@
   <dimension ref="A1:H220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="1" max="8" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -7730,7 +7723,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -8009,7 +8002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25110,7 +25103,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -26783,13 +26776,13 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -27112,7 +27105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF3CE7-E34E-044F-A5DE-BB3AC931C52F}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Update manifest with polished Home tab button
- Updated to black PF logo (visible on light/dark backgrounds)
- Button label: 'Launch TaiTools'
- Group label: 'TaiTools'
- Consistent branding with ACPTools
</commit_message>
<xml_diff>
--- a/Excel Templates/ForgeSuite_Template_Tai.xlsx
+++ b/Excel Templates/ForgeSuite_Template_Tai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.paeth/Customer-Tai-Software/Excel Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF721AA-2E74-2D4B-8582-E9644CDA9644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3D2B73-73ED-B346-B969-7075AAFCBF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" activeTab="3" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34560" windowHeight="20180" xr2:uid="{DC999B35-613C-7448-8BDE-5A2B7D076032}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_Homepage" sheetId="2" r:id="rId1"/>
@@ -3156,7 +3156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF8234F-E74B-4C4C-B812-7718B620274B}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8352,7 +8354,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A232" sqref="A232:A468"/>
+      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44390,7 +44392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A1350D-BBEB-BD4B-9908-B0A7FABAE65A}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>

</xml_diff>